<commit_message>
Color code for Alerts
</commit_message>
<xml_diff>
--- a/data/nifty_options/nifty_options_2026-01.xlsx
+++ b/data/nifty_options/nifty_options_2026-01.xlsx
@@ -20,7 +20,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -39,10 +39,26 @@
     </font>
     <font>
       <b val="1"/>
-      <color rgb="009C6500"/>
+      <color rgb="00006100"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00375623"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00974806"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="009C0006"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill/>
     </fill>
@@ -57,8 +73,38 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFEB9C"/>
-        <bgColor rgb="00FFEB9C"/>
+        <fgColor rgb="00C6EFCE"/>
+        <bgColor rgb="00C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000B050"/>
+        <bgColor rgb="0000B050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0092D050"/>
+        <bgColor rgb="0092D050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC000"/>
+        <bgColor rgb="00FFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC7CE"/>
+        <bgColor rgb="00FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -80,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -91,6 +137,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -98,6 +147,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -465,7 +526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -477,28 +538,34 @@
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
     <col width="8" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="8" customWidth="1" min="6" max="6"/>
-    <col width="10" customWidth="1" min="7" max="7"/>
-    <col width="14" customWidth="1" min="8" max="8"/>
-    <col width="12" customWidth="1" min="9" max="9"/>
-    <col width="16" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="8" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="10" max="10"/>
     <col width="10" customWidth="1" min="11" max="11"/>
-    <col width="12" customWidth="1" min="12" max="12"/>
-    <col width="12" customWidth="1" min="13" max="13"/>
-    <col width="14" customWidth="1" min="14" max="14"/>
-    <col width="12" customWidth="1" min="15" max="15"/>
-    <col width="16" customWidth="1" min="16" max="16"/>
-    <col width="16" customWidth="1" min="17" max="17"/>
-    <col width="14" customWidth="1" min="18" max="18"/>
-    <col width="14" customWidth="1" min="19" max="19"/>
-    <col width="16" customWidth="1" min="20" max="20"/>
-    <col width="14" customWidth="1" min="21" max="21"/>
-    <col width="14" customWidth="1" min="22" max="22"/>
-    <col width="40" customWidth="1" min="23" max="23"/>
-    <col width="40" customWidth="1" min="24" max="24"/>
-    <col width="12" customWidth="1" min="25" max="25"/>
+    <col width="10" customWidth="1" min="12" max="12"/>
+    <col width="14" customWidth="1" min="13" max="13"/>
+    <col width="12" customWidth="1" min="14" max="14"/>
+    <col width="16" customWidth="1" min="15" max="15"/>
+    <col width="10" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="17" max="17"/>
+    <col width="12" customWidth="1" min="18" max="18"/>
+    <col width="12" customWidth="1" min="19" max="19"/>
+    <col width="14" customWidth="1" min="20" max="20"/>
+    <col width="12" customWidth="1" min="21" max="21"/>
+    <col width="16" customWidth="1" min="22" max="22"/>
+    <col width="16" customWidth="1" min="23" max="23"/>
+    <col width="14" customWidth="1" min="24" max="24"/>
+    <col width="14" customWidth="1" min="25" max="25"/>
+    <col width="16" customWidth="1" min="26" max="26"/>
+    <col width="14" customWidth="1" min="27" max="27"/>
+    <col width="14" customWidth="1" min="28" max="28"/>
+    <col width="40" customWidth="1" min="29" max="29"/>
+    <col width="40" customWidth="1" min="30" max="30"/>
+    <col width="12" customWidth="1" min="31" max="31"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -519,110 +586,140 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Signal_Tier</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Position_Size</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Premium_Quality</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Total_Score</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>NIFTY_Spot</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>VIX</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>VIX_Trend</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>VIX_Score</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>IV_Rank</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Market_Regime</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Regime_Score</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>OI_Pattern</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>OI_Score</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Theta_Score</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Gamma_Score</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Vega_Score</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Best_Strategy</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Expiry_1</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Days_To_Expiry_1</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Straddle_Premium</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Straddle_Theta</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Straddle_Gamma</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Strangle_Premium</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Strangle_Theta</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Strangle_Gamma</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Recommendation</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Risk_Factors</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Telegram_Sent</t>
         </is>
@@ -631,97 +728,484 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>11:59:05</t>
+          <t>14:24:27</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>62</v>
-      </c>
-      <c r="E2" s="4" t="n">
-        <v>26146.05</v>
-      </c>
-      <c r="F2" s="4" t="n">
-        <v>9.23</v>
-      </c>
-      <c r="G2" s="4" t="n">
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>SELL_STRONG</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>EXCELLENT</t>
+        </is>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>85</v>
+      </c>
+      <c r="H2" s="6" t="n">
+        <v>21850.5</v>
+      </c>
+      <c r="I2" s="6" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="J2" s="6" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="K2" s="5" t="n">
+        <v>60</v>
+      </c>
+      <c r="L2" s="5" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="M2" s="2" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="N2" s="5" t="n">
         <v>100</v>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="O2" s="2" t="inlineStr">
+        <is>
+          <t>LONG_UNWINDING</t>
+        </is>
+      </c>
+      <c r="P2" s="5" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="R2" s="5" t="n">
+        <v>85</v>
+      </c>
+      <c r="S2" s="5" t="n">
+        <v>75</v>
+      </c>
+      <c r="T2" s="2" t="inlineStr">
+        <is>
+          <t>STRADDLE</t>
+        </is>
+      </c>
+      <c r="U2" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="V2" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="W2" s="6" t="n">
+        <v>355</v>
+      </c>
+      <c r="X2" s="6" t="n">
+        <v>45</v>
+      </c>
+      <c r="Y2" s="7" t="n">
+        <v>0.0012</v>
+      </c>
+      <c r="Z2" s="6" t="n">
+        <v>185</v>
+      </c>
+      <c r="AA2" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB2" s="7" t="n">
+        <v>0.0008</v>
+      </c>
+      <c r="AC2" s="2" t="inlineStr">
+        <is>
+          <t>Test scenario 1</t>
+        </is>
+      </c>
+      <c r="AD2" s="2" t="inlineStr">
+        <is>
+          <t>Test risk</t>
+        </is>
+      </c>
+      <c r="AE2" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-03</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>14:24:27</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D3" s="8" t="inlineStr">
+        <is>
+          <t>SELL_MODERATE</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>75%</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>72</v>
+      </c>
+      <c r="H3" s="6" t="n">
+        <v>21850.5</v>
+      </c>
+      <c r="I3" s="6" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="J3" s="6" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="K3" s="5" t="n">
+        <v>60</v>
+      </c>
+      <c r="L3" s="5" t="n">
+        <v>18.2</v>
+      </c>
+      <c r="M3" s="2" t="inlineStr">
         <is>
           <t>NEUTRAL</t>
         </is>
       </c>
-      <c r="I2" s="4" t="n">
+      <c r="N3" s="5" t="n">
         <v>100</v>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="O3" s="2" t="inlineStr">
         <is>
           <t>LONG_UNWINDING</t>
         </is>
       </c>
-      <c r="K2" s="4" t="n">
+      <c r="P3" s="5" t="n">
         <v>70</v>
       </c>
-      <c r="L2" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="M2" s="4" t="n">
-        <v>50</v>
-      </c>
-      <c r="N2" s="2" t="inlineStr">
+      <c r="Q3" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="R3" s="5" t="n">
+        <v>85</v>
+      </c>
+      <c r="S3" s="5" t="n">
+        <v>75</v>
+      </c>
+      <c r="T3" s="2" t="inlineStr">
         <is>
           <t>STRADDLE</t>
         </is>
       </c>
-      <c r="O2" s="2" t="inlineStr">
-        <is>
-          <t>2026-01-06</t>
-        </is>
-      </c>
-      <c r="P2" s="2" t="n">
+      <c r="U3" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="V3" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="W3" s="6" t="n">
+        <v>355</v>
+      </c>
+      <c r="X3" s="6" t="n">
+        <v>45</v>
+      </c>
+      <c r="Y3" s="7" t="n">
+        <v>0.0012</v>
+      </c>
+      <c r="Z3" s="6" t="n">
+        <v>185</v>
+      </c>
+      <c r="AA3" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB3" s="7" t="n">
+        <v>0.0008</v>
+      </c>
+      <c r="AC3" s="2" t="inlineStr">
+        <is>
+          <t>Test scenario 2</t>
+        </is>
+      </c>
+      <c r="AD3" s="2" t="inlineStr">
+        <is>
+          <t>Test risk</t>
+        </is>
+      </c>
+      <c r="AE3" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-03</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>14:24:27</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D4" s="9" t="inlineStr">
+        <is>
+          <t>SELL_WEAK</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>BELOW AVERAGE</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>65</v>
+      </c>
+      <c r="H4" s="6" t="n">
+        <v>21850.5</v>
+      </c>
+      <c r="I4" s="6" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="J4" s="6" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="K4" s="5" t="n">
+        <v>60</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="M4" s="2" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="N4" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="O4" s="2" t="inlineStr">
+        <is>
+          <t>LONG_UNWINDING</t>
+        </is>
+      </c>
+      <c r="P4" s="5" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q4" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="R4" s="5" t="n">
+        <v>85</v>
+      </c>
+      <c r="S4" s="5" t="n">
+        <v>75</v>
+      </c>
+      <c r="T4" s="2" t="inlineStr">
+        <is>
+          <t>STRADDLE</t>
+        </is>
+      </c>
+      <c r="U4" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="V4" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="W4" s="6" t="n">
+        <v>355</v>
+      </c>
+      <c r="X4" s="6" t="n">
+        <v>45</v>
+      </c>
+      <c r="Y4" s="7" t="n">
+        <v>0.0012</v>
+      </c>
+      <c r="Z4" s="6" t="n">
+        <v>185</v>
+      </c>
+      <c r="AA4" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB4" s="7" t="n">
+        <v>0.0008</v>
+      </c>
+      <c r="AC4" s="2" t="inlineStr">
+        <is>
+          <t>Test scenario 3</t>
+        </is>
+      </c>
+      <c r="AD4" s="2" t="inlineStr">
+        <is>
+          <t>Test risk</t>
+        </is>
+      </c>
+      <c r="AE4" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-03</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>14:24:27</t>
+        </is>
+      </c>
+      <c r="C5" s="10" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D5" s="11" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>CHEAP</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="H5" s="6" t="n">
+        <v>21850.5</v>
+      </c>
+      <c r="I5" s="6" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="J5" s="6" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="K5" s="5" t="n">
+        <v>60</v>
+      </c>
+      <c r="L5" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="Q2" s="5" t="n">
-        <v>492.55</v>
-      </c>
-      <c r="R2" s="5" t="n">
-        <v>5.01</v>
-      </c>
-      <c r="S2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" s="5" t="n">
-        <v>400.9</v>
-      </c>
-      <c r="U2" s="5" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="V2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="W2" s="2" t="inlineStr">
-        <is>
-          <t>Mixed conditions, wait for better setup</t>
-        </is>
-      </c>
-      <c r="X2" s="2" t="inlineStr">
-        <is>
-          <t>No significant risks identified</t>
-        </is>
-      </c>
-      <c r="Y2" s="2" t="inlineStr">
-        <is>
-          <t>No</t>
+      <c r="M5" s="2" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="N5" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="O5" s="2" t="inlineStr">
+        <is>
+          <t>LONG_UNWINDING</t>
+        </is>
+      </c>
+      <c r="P5" s="5" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q5" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="R5" s="5" t="n">
+        <v>85</v>
+      </c>
+      <c r="S5" s="5" t="n">
+        <v>75</v>
+      </c>
+      <c r="T5" s="2" t="inlineStr">
+        <is>
+          <t>STRADDLE</t>
+        </is>
+      </c>
+      <c r="U5" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="V5" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="W5" s="6" t="n">
+        <v>355</v>
+      </c>
+      <c r="X5" s="6" t="n">
+        <v>45</v>
+      </c>
+      <c r="Y5" s="7" t="n">
+        <v>0.0012</v>
+      </c>
+      <c r="Z5" s="6" t="n">
+        <v>185</v>
+      </c>
+      <c r="AA5" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB5" s="7" t="n">
+        <v>0.0008</v>
+      </c>
+      <c r="AC5" s="2" t="inlineStr">
+        <is>
+          <t>Test scenario 4</t>
+        </is>
+      </c>
+      <c r="AD5" s="2" t="inlineStr">
+        <is>
+          <t>Test risk</t>
+        </is>
+      </c>
+      <c r="AE5" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add CPR First Touch Alert System with 1-min NIFTY monitoring
- Create cpr_state_tracker.py: State persistence with crossing detection
- Create cpr_first_touch_monitor.py: Main monitoring service (1-min cycle)
- Add LaunchD service: com.nse.cpr.monitor.plist + cpr_service.sh
- Implement cache sharing: CPR writes 1-min NIFTY data, options analyzer reads
- Add config parameters: ENABLE_CPR_ALERTS, CPR_DRY_RUN_MODE, cooldown
- Modify nifty_option_analyzer.py: Use cached NIFTY data (saves ~22 API calls/day)
- Alert on first touch of TC/BC levels with direction (FROM_ABOVE/FROM_BELOW)
- 24-hour cooldown prevents duplicate alerts

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/nifty_options/nifty_options_2026-01.xlsx
+++ b/data/nifty_options/nifty_options_2026-01.xlsx
@@ -526,7 +526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE13"/>
+  <dimension ref="A1:AE14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2161,6 +2161,127 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-12</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>10:00:13</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="inlineStr">
+        <is>
+          <t>SELL_STRONG</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>EXCELLENT</t>
+        </is>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>85.59999999999999</v>
+      </c>
+      <c r="H14" s="6" t="n">
+        <v>25559.65</v>
+      </c>
+      <c r="I14" s="6" t="n">
+        <v>11.82</v>
+      </c>
+      <c r="J14" s="6" t="n">
+        <v>1.87</v>
+      </c>
+      <c r="K14" s="5" t="n">
+        <v>90.59999999999999</v>
+      </c>
+      <c r="L14" s="5" t="n">
+        <v>34.2</v>
+      </c>
+      <c r="M14" s="2" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="N14" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="O14" s="2" t="inlineStr">
+        <is>
+          <t>LONG_UNWINDING</t>
+        </is>
+      </c>
+      <c r="P14" s="5" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q14" s="5" t="n">
+        <v>75.59999999999999</v>
+      </c>
+      <c r="R14" s="5" t="n">
+        <v>89.5</v>
+      </c>
+      <c r="S14" s="5" t="n">
+        <v>86.2</v>
+      </c>
+      <c r="T14" s="2" t="inlineStr">
+        <is>
+          <t>STRADDLE</t>
+        </is>
+      </c>
+      <c r="U14" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="V14" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="W14" s="6" t="n">
+        <v>348.25</v>
+      </c>
+      <c r="X14" s="6" t="n">
+        <v>37.81</v>
+      </c>
+      <c r="Y14" s="7" t="n">
+        <v>0.00105</v>
+      </c>
+      <c r="Z14" s="6" t="n">
+        <v>257.9</v>
+      </c>
+      <c r="AA14" s="6" t="n">
+        <v>37.51</v>
+      </c>
+      <c r="AB14" s="7" t="n">
+        <v>0.001041</v>
+      </c>
+      <c r="AC14" s="2" t="inlineStr">
+        <is>
+          <t>Excellent conditions for option selling</t>
+        </is>
+      </c>
+      <c r="AD14" s="2" t="inlineStr">
+        <is>
+          <t>VIX rising (+1.9 points) - conditions deteriorating</t>
+        </is>
+      </c>
+      <c r="AE14" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix CPR alert state persistence bug + trading-day-based cooldown
Critical bug fixes:
- Fix state reset issue: Monitor now checks persistent state file instead of in-memory cache
- Replace 24-hour cooldown with trading-day-based reset (9:15 AM each day)
- Add cache update to get_multiple_instruments for NIFTY data sharing
- Fix method name: update_quotes → set_cached_quotes in api_coordinator

State persistence now works correctly:
- Previous position preserved across 1-minute monitor cycles
- Crossing detection working: FROM_ABOVE/FROM_BELOW alerts
- Alert flags reset at market open, not 24h from alert time

Testing confirmed:
- State tracker persists across process restarts
- Crossings detected correctly in test simulation
- Ready for production testing tomorrow during market hours

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/nifty_options/nifty_options_2026-01.xlsx
+++ b/data/nifty_options/nifty_options_2026-01.xlsx
@@ -526,7 +526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE14"/>
+  <dimension ref="A1:AE19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2282,6 +2282,603 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-13</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>10:00:11</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D15" s="4" t="inlineStr">
+        <is>
+          <t>SELL_STRONG</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>EXCELLENT</t>
+        </is>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>89.5</v>
+      </c>
+      <c r="H15" s="6" t="n">
+        <v>25709.4</v>
+      </c>
+      <c r="I15" s="6" t="n">
+        <v>11.67</v>
+      </c>
+      <c r="J15" s="6" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="K15" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="L15" s="5" t="n">
+        <v>30.1</v>
+      </c>
+      <c r="M15" s="2" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="N15" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="O15" s="2" t="inlineStr">
+        <is>
+          <t>LONG_UNWINDING</t>
+        </is>
+      </c>
+      <c r="P15" s="5" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q15" s="5" t="n">
+        <v>81.3</v>
+      </c>
+      <c r="R15" s="5" t="n">
+        <v>88.8</v>
+      </c>
+      <c r="S15" s="5" t="n">
+        <v>90</v>
+      </c>
+      <c r="T15" s="2" t="inlineStr">
+        <is>
+          <t>STRADDLE</t>
+        </is>
+      </c>
+      <c r="U15" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="V15" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="W15" s="6" t="n">
+        <v>328.9</v>
+      </c>
+      <c r="X15" s="6" t="n">
+        <v>40.66</v>
+      </c>
+      <c r="Y15" s="7" t="n">
+        <v>0.001118</v>
+      </c>
+      <c r="Z15" s="6" t="n">
+        <v>239.7</v>
+      </c>
+      <c r="AA15" s="6" t="n">
+        <v>40.28</v>
+      </c>
+      <c r="AB15" s="7" t="n">
+        <v>0.001106</v>
+      </c>
+      <c r="AC15" s="2" t="inlineStr">
+        <is>
+          <t>Excellent conditions for option selling</t>
+        </is>
+      </c>
+      <c r="AD15" s="2" t="inlineStr">
+        <is>
+          <t>No significant risks identified</t>
+        </is>
+      </c>
+      <c r="AE15" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-13</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>12:15:08</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D16" s="4" t="inlineStr">
+        <is>
+          <t>SELL_STRONG</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>EXCELLENT</t>
+        </is>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>86.5</v>
+      </c>
+      <c r="H16" s="6" t="n">
+        <v>25711.85</v>
+      </c>
+      <c r="I16" s="6" t="n">
+        <v>11.43</v>
+      </c>
+      <c r="J16" s="6" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="K16" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="L16" s="5" t="n">
+        <v>27.1</v>
+      </c>
+      <c r="M16" s="2" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="N16" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="O16" s="2" t="inlineStr">
+        <is>
+          <t>SHORT_BUILDUP</t>
+        </is>
+      </c>
+      <c r="P16" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q16" s="5" t="n">
+        <v>81.3</v>
+      </c>
+      <c r="R16" s="5" t="n">
+        <v>88.8</v>
+      </c>
+      <c r="S16" s="5" t="n">
+        <v>90</v>
+      </c>
+      <c r="T16" s="2" t="inlineStr">
+        <is>
+          <t>STRADDLE</t>
+        </is>
+      </c>
+      <c r="U16" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="V16" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="W16" s="6" t="n">
+        <v>312.05</v>
+      </c>
+      <c r="X16" s="6" t="n">
+        <v>40.66</v>
+      </c>
+      <c r="Y16" s="7" t="n">
+        <v>0.001116</v>
+      </c>
+      <c r="Z16" s="6" t="n">
+        <v>222.1</v>
+      </c>
+      <c r="AA16" s="6" t="n">
+        <v>40.28</v>
+      </c>
+      <c r="AB16" s="7" t="n">
+        <v>0.001106</v>
+      </c>
+      <c r="AC16" s="2" t="inlineStr">
+        <is>
+          <t>Excellent conditions for option selling</t>
+        </is>
+      </c>
+      <c r="AD16" s="2" t="inlineStr">
+        <is>
+          <t>Strong OI buildup (SHORT_BUILDUP) - momentum trade</t>
+        </is>
+      </c>
+      <c r="AE16" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-13</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>14:45:14</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D17" s="8" t="inlineStr">
+        <is>
+          <t>SELL_MODERATE</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>75%</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>82.8</v>
+      </c>
+      <c r="H17" s="6" t="n">
+        <v>25696.1</v>
+      </c>
+      <c r="I17" s="6" t="n">
+        <v>11.36</v>
+      </c>
+      <c r="J17" s="6" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="K17" s="5" t="n">
+        <v>85</v>
+      </c>
+      <c r="L17" s="5" t="n">
+        <v>24.9</v>
+      </c>
+      <c r="M17" s="2" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="N17" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="O17" s="2" t="inlineStr">
+        <is>
+          <t>SHORT_BUILDUP</t>
+        </is>
+      </c>
+      <c r="P17" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q17" s="5" t="n">
+        <v>81.2</v>
+      </c>
+      <c r="R17" s="5" t="n">
+        <v>88.8</v>
+      </c>
+      <c r="S17" s="5" t="n">
+        <v>90</v>
+      </c>
+      <c r="T17" s="2" t="inlineStr">
+        <is>
+          <t>STRADDLE</t>
+        </is>
+      </c>
+      <c r="U17" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="V17" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="W17" s="6" t="n">
+        <v>290</v>
+      </c>
+      <c r="X17" s="6" t="n">
+        <v>40.61</v>
+      </c>
+      <c r="Y17" s="7" t="n">
+        <v>0.00112</v>
+      </c>
+      <c r="Z17" s="6" t="n">
+        <v>203.1</v>
+      </c>
+      <c r="AA17" s="6" t="n">
+        <v>40.23</v>
+      </c>
+      <c r="AB17" s="7" t="n">
+        <v>0.001109</v>
+      </c>
+      <c r="AC17" s="2" t="inlineStr">
+        <is>
+          <t>Excellent conditions for option selling</t>
+        </is>
+      </c>
+      <c r="AD17" s="2" t="inlineStr">
+        <is>
+          <t>Low IV Rank (24.9%) - premiums historically cheap, poor value for selling; Strong OI buildup (SHORT_BUILDUP) - momentum trade</t>
+        </is>
+      </c>
+      <c r="AE17" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-14</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>10:00:13</t>
+        </is>
+      </c>
+      <c r="C18" s="10" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D18" s="11" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G18" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="6" t="n">
+        <v>25731.3</v>
+      </c>
+      <c r="I18" s="6" t="n">
+        <v>11.24</v>
+      </c>
+      <c r="J18" s="6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="K18" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="5" t="n">
+        <v>23.7</v>
+      </c>
+      <c r="M18" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N18" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P18" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U18" s="2" t="inlineStr"/>
+      <c r="V18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25731.30 below BC 25751.55 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD18" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25731.30 below BC 25751.55 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE18" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-15</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>10:00:12</t>
+        </is>
+      </c>
+      <c r="C19" s="10" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D19" s="11" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="6" t="n">
+        <v>25665.6</v>
+      </c>
+      <c r="I19" s="6" t="n">
+        <v>11.32</v>
+      </c>
+      <c r="J19" s="6" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="K19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="5" t="n">
+        <v>25.2</v>
+      </c>
+      <c r="M19" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U19" s="2" t="inlineStr"/>
+      <c r="V19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25665.60 below BC 25751.55 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD19" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25665.60 below BC 25751.55 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE19" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix 5-min/10-min alerts: reload LaunchAgent + sector EOD report
- Reloaded com.nse.stockmonitor.plist (was inactive)
- Added sector analysis enhancements
- Updated config for CPR alerts
- Database and cache updates from monitoring

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/nifty_options/nifty_options_2026-01.xlsx
+++ b/data/nifty_options/nifty_options_2026-01.xlsx
@@ -526,7 +526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE19"/>
+  <dimension ref="A1:AE20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2879,6 +2879,123 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-16</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>10:00:11</t>
+        </is>
+      </c>
+      <c r="C20" s="10" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D20" s="11" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="6" t="n">
+        <v>25739.05</v>
+      </c>
+      <c r="I20" s="6" t="n">
+        <v>11.16</v>
+      </c>
+      <c r="J20" s="6" t="n">
+        <v>-0.21</v>
+      </c>
+      <c r="K20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="5" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="M20" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U20" s="2" t="inlineStr"/>
+      <c r="V20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25739.05 above TC 25676.35 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD20" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25739.05 above TC 25676.35 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE20" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add service health dashboard + data accuracy improvements
- Add service_health.py: centralized health tracking for all services
- Add health_dashboard.py: troubleshooting dashboard with --watch mode
- Update onemin_monitor.py: report errors to health tracker, API fallback with logging
- Update price_cache.py: fail explicitly on data issues instead of silent fallback
- Data accuracy > graceful degradation: errors are now visible, not hidden

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/nifty_options/nifty_options_2026-01.xlsx
+++ b/data/nifty_options/nifty_options_2026-01.xlsx
@@ -526,7 +526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE20"/>
+  <dimension ref="A1:AE21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2996,6 +2996,123 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-19</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>10:00:08</t>
+        </is>
+      </c>
+      <c r="C21" s="10" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D21" s="11" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G21" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="6" t="n">
+        <v>25539.9</v>
+      </c>
+      <c r="I21" s="6" t="n">
+        <v>11.98</v>
+      </c>
+      <c r="J21" s="6" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="K21" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" s="5" t="n">
+        <v>39.6</v>
+      </c>
+      <c r="M21" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N21" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P21" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U21" s="2" t="inlineStr"/>
+      <c r="V21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25539.90 below BC 25767.95 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD21" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25539.90 below BC 25767.95 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE21" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Migrate services to central DB + fix configs
- Add central_db_reader.py shared helper with freshness checks + API fallback
- Migrate stock_monitor, sector_analyzer, nifty_option_analyzer to central DB
- Migrate cpr_first_touch_monitor, price_action_monitor to central DB
- Increase PRICE_ACTION_MIN_CONFIDENCE to 8.0 (high confidence only)
- Remove NIFTYNXT50 from fo_stocks.json (it's an index, not stock)
- Add Jan 15, 2026 holiday (Municipal Corporation Elections)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/nifty_options/nifty_options_2026-01.xlsx
+++ b/data/nifty_options/nifty_options_2026-01.xlsx
@@ -526,7 +526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE21"/>
+  <dimension ref="A1:AE22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3113,6 +3113,123 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>10:00:07</t>
+        </is>
+      </c>
+      <c r="C22" s="10" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D22" s="11" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="6" t="n">
+        <v>25458</v>
+      </c>
+      <c r="I22" s="6" t="n">
+        <v>12.3</v>
+      </c>
+      <c r="J22" s="6" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="K22" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" s="5" t="n">
+        <v>45.9</v>
+      </c>
+      <c r="M22" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N22" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P22" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U22" s="2" t="inlineStr"/>
+      <c r="V22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W22" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X22" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25458.00 below BC 25573.82 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD22" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25458.00 below BC 25573.82 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE22" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data files + cache - 2026-01-22
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/nifty_options/nifty_options_2026-01.xlsx
+++ b/data/nifty_options/nifty_options_2026-01.xlsx
@@ -526,7 +526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE22"/>
+  <dimension ref="A1:AE24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3230,6 +3230,240 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-21</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>10:00:09</t>
+        </is>
+      </c>
+      <c r="C23" s="10" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D23" s="11" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="6" t="n">
+        <v>25157.4</v>
+      </c>
+      <c r="I23" s="6" t="n">
+        <v>13.16</v>
+      </c>
+      <c r="J23" s="6" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="K23" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" s="5" t="n">
+        <v>53.9</v>
+      </c>
+      <c r="M23" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N23" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P23" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T23" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U23" s="2" t="inlineStr"/>
+      <c r="V23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W23" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X23" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25157.40 below BC 25378.17 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD23" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25157.40 below BC 25378.17 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE23" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>10:00:08</t>
+        </is>
+      </c>
+      <c r="C24" s="10" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D24" s="11" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="6" t="n">
+        <v>25397.4</v>
+      </c>
+      <c r="I24" s="6" t="n">
+        <v>13.47</v>
+      </c>
+      <c r="J24" s="6" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="K24" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="5" t="n">
+        <v>56.7</v>
+      </c>
+      <c r="M24" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N24" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P24" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U24" s="2" t="inlineStr"/>
+      <c r="V24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W24" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X24" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25397.40 above TC 25141.79 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD24" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25397.40 above TC 25141.79 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE24" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix missing _send_message method in TelegramNotifier
Add _send_message() method to TelegramNotifier facade class.
Called by main.py, token_manager.py, and greeks_difference_tracker.py
for sending warning/status messages.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/nifty_options/nifty_options_2026-01.xlsx
+++ b/data/nifty_options/nifty_options_2026-01.xlsx
@@ -526,7 +526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE24"/>
+  <dimension ref="A1:AE25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3464,6 +3464,123 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-23</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>10:00:07</t>
+        </is>
+      </c>
+      <c r="C25" s="10" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D25" s="11" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="6" t="n">
+        <v>25292.7</v>
+      </c>
+      <c r="I25" s="6" t="n">
+        <v>13.63</v>
+      </c>
+      <c r="J25" s="6" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="K25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="5" t="n">
+        <v>58.5</v>
+      </c>
+      <c r="M25" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U25" s="2" t="inlineStr"/>
+      <c r="V25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W25" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X25" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25292.70 below BC 25302.12 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD25" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25292.70 below BC 25302.12 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE25" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data files + cache - 2026-01-29
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/nifty_options/nifty_options_2026-01.xlsx
+++ b/data/nifty_options/nifty_options_2026-01.xlsx
@@ -526,7 +526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE25"/>
+  <dimension ref="A1:AE27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3581,6 +3581,240 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>10:00:09</t>
+        </is>
+      </c>
+      <c r="C26" s="10" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D26" s="11" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G26" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="6" t="n">
+        <v>25117.55</v>
+      </c>
+      <c r="I26" s="6" t="n">
+        <v>15.42</v>
+      </c>
+      <c r="J26" s="6" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="K26" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" s="5" t="n">
+        <v>78.7</v>
+      </c>
+      <c r="M26" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N26" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P26" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T26" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U26" s="2" t="inlineStr"/>
+      <c r="V26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W26" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X26" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25117.55 above TC 25094.64 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD26" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25117.55 above TC 25094.64 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE26" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>10:00:14</t>
+        </is>
+      </c>
+      <c r="C27" s="10" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D27" s="11" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G27" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="6" t="n">
+        <v>25187.9</v>
+      </c>
+      <c r="I27" s="6" t="n">
+        <v>13.99</v>
+      </c>
+      <c r="J27" s="6" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="K27" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="5" t="n">
+        <v>65.59999999999999</v>
+      </c>
+      <c r="M27" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N27" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P27" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U27" s="2" t="inlineStr"/>
+      <c r="V27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X27" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25187.90 below BC 25279.88 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD27" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25187.90 below BC 25279.88 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE27" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data files + cache - 2026-01-30
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/nifty_options/nifty_options_2026-01.xlsx
+++ b/data/nifty_options/nifty_options_2026-01.xlsx
@@ -526,7 +526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE27"/>
+  <dimension ref="A1:AE30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3815,6 +3815,365 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>10:00:11</t>
+        </is>
+      </c>
+      <c r="C28" s="10" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D28" s="11" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="6" t="n">
+        <v>25284.7</v>
+      </c>
+      <c r="I28" s="6" t="n">
+        <v>13.84</v>
+      </c>
+      <c r="J28" s="6" t="n">
+        <v>-0.61</v>
+      </c>
+      <c r="K28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="5" t="n">
+        <v>65.59999999999999</v>
+      </c>
+      <c r="M28" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U28" s="2" t="inlineStr"/>
+      <c r="V28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X28" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25284.70 below BC 25308.97 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD28" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25284.70 below BC 25308.97 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE28" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>10:15:12</t>
+        </is>
+      </c>
+      <c r="C29" s="3" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D29" s="4" t="inlineStr">
+        <is>
+          <t>SELL_STRONG</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>EXCELLENT</t>
+        </is>
+      </c>
+      <c r="G29" s="5" t="n">
+        <v>80.2</v>
+      </c>
+      <c r="H29" s="6" t="n">
+        <v>25317</v>
+      </c>
+      <c r="I29" s="6" t="n">
+        <v>13.73</v>
+      </c>
+      <c r="J29" s="6" t="n">
+        <v>-0.72</v>
+      </c>
+      <c r="K29" s="5" t="n">
+        <v>75</v>
+      </c>
+      <c r="L29" s="5" t="n">
+        <v>62.6</v>
+      </c>
+      <c r="M29" s="2" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="N29" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="O29" s="2" t="inlineStr">
+        <is>
+          <t>LONG_UNWINDING</t>
+        </is>
+      </c>
+      <c r="P29" s="5" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q29" s="5" t="n">
+        <v>63.9</v>
+      </c>
+      <c r="R29" s="5" t="n">
+        <v>91</v>
+      </c>
+      <c r="S29" s="5" t="n">
+        <v>90</v>
+      </c>
+      <c r="T29" s="2" t="inlineStr">
+        <is>
+          <t>STRADDLE</t>
+        </is>
+      </c>
+      <c r="U29" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="V29" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="W29" s="6" t="n">
+        <v>537.15</v>
+      </c>
+      <c r="X29" s="6" t="n">
+        <v>31.97</v>
+      </c>
+      <c r="Y29" s="7" t="n">
+        <v>0.000904</v>
+      </c>
+      <c r="Z29" s="6" t="n">
+        <v>444.8</v>
+      </c>
+      <c r="AA29" s="6" t="n">
+        <v>31.78</v>
+      </c>
+      <c r="AB29" s="7" t="n">
+        <v>0.000898</v>
+      </c>
+      <c r="AC29" s="2" t="inlineStr">
+        <is>
+          <t>Excellent conditions for option selling</t>
+        </is>
+      </c>
+      <c r="AD29" s="2" t="inlineStr">
+        <is>
+          <t>No significant risks identified</t>
+        </is>
+      </c>
+      <c r="AE29" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>14:00:11</t>
+        </is>
+      </c>
+      <c r="C30" s="3" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D30" s="4" t="inlineStr">
+        <is>
+          <t>SELL_STRONG</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>EXCELLENT</t>
+        </is>
+      </c>
+      <c r="G30" s="5" t="n">
+        <v>80.2</v>
+      </c>
+      <c r="H30" s="6" t="n">
+        <v>25344.6</v>
+      </c>
+      <c r="I30" s="6" t="n">
+        <v>13.78</v>
+      </c>
+      <c r="J30" s="6" t="n">
+        <v>-0.67</v>
+      </c>
+      <c r="K30" s="5" t="n">
+        <v>75</v>
+      </c>
+      <c r="L30" s="5" t="n">
+        <v>64.09999999999999</v>
+      </c>
+      <c r="M30" s="2" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="N30" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="O30" s="2" t="inlineStr">
+        <is>
+          <t>SHORT_COVERING</t>
+        </is>
+      </c>
+      <c r="P30" s="5" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q30" s="5" t="n">
+        <v>63.9</v>
+      </c>
+      <c r="R30" s="5" t="n">
+        <v>91</v>
+      </c>
+      <c r="S30" s="5" t="n">
+        <v>90</v>
+      </c>
+      <c r="T30" s="2" t="inlineStr">
+        <is>
+          <t>STRADDLE</t>
+        </is>
+      </c>
+      <c r="U30" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="V30" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="W30" s="6" t="n">
+        <v>544.45</v>
+      </c>
+      <c r="X30" s="6" t="n">
+        <v>31.97</v>
+      </c>
+      <c r="Y30" s="7" t="n">
+        <v>0.000904</v>
+      </c>
+      <c r="Z30" s="6" t="n">
+        <v>452.7</v>
+      </c>
+      <c r="AA30" s="6" t="n">
+        <v>31.79</v>
+      </c>
+      <c r="AB30" s="7" t="n">
+        <v>0.000899</v>
+      </c>
+      <c r="AC30" s="2" t="inlineStr">
+        <is>
+          <t>Excellent conditions for option selling</t>
+        </is>
+      </c>
+      <c r="AD30" s="2" t="inlineStr">
+        <is>
+          <t>No significant risks identified</t>
+        </is>
+      </c>
+      <c r="AE30" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>